<commit_message>
lodoss war product codes
</commit_message>
<xml_diff>
--- a/record-of-lodoss-war/checklist.xlsx
+++ b/record-of-lodoss-war/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/record-of-lodoss-war/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9697E2A6-3738-5147-BE43-DFB494E6B7AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977282D9-2044-DC46-91FD-B7C0810E237C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{3EE3A57C-8E29-5448-9F58-6C32800A81B4}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{3EE3A57C-8E29-5448-9F58-6C32800A81B4}"/>
   </bookViews>
   <sheets>
     <sheet name="checklist" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
   <si>
     <t>year</t>
   </si>
@@ -204,6 +204,24 @@
   </si>
   <si>
     <t>scenario</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>6-41</t>
+  </si>
+  <si>
+    <t>6-42</t>
+  </si>
+  <si>
+    <t>6-43</t>
+  </si>
+  <si>
+    <t>885-2</t>
+  </si>
+  <si>
+    <t>885-5</t>
   </si>
 </sst>
 </file>
@@ -253,9 +271,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C9804C8-627B-F645-81DF-9E8F0046BE23}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="A8:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -584,7 +603,7 @@
     <col min="5" max="5" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -603,8 +622,11 @@
       <c r="F1" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1989</v>
       </c>
@@ -623,8 +645,9 @@
       <c r="F2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1991</v>
       </c>
@@ -643,8 +666,9 @@
       <c r="F3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1994</v>
       </c>
@@ -663,8 +687,9 @@
       <c r="F4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1995</v>
       </c>
@@ -683,8 +708,11 @@
       <c r="F5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1996</v>
       </c>
@@ -703,8 +731,11 @@
       <c r="F6" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1998</v>
       </c>
@@ -723,8 +754,9 @@
       <c r="F7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1995</v>
       </c>
@@ -743,8 +775,9 @@
       <c r="F8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1989</v>
       </c>
@@ -763,8 +796,9 @@
       <c r="F9" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1990</v>
       </c>
@@ -783,8 +817,9 @@
       <c r="F10" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1991</v>
       </c>
@@ -803,8 +838,9 @@
       <c r="F11" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -820,8 +856,9 @@
       <c r="F12" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -837,8 +874,9 @@
       <c r="F13" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -854,8 +892,9 @@
       <c r="F14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1998</v>
       </c>
@@ -874,8 +913,11 @@
       <c r="F15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1998</v>
       </c>
@@ -894,8 +936,11 @@
       <c r="F16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1998</v>
       </c>
@@ -914,8 +959,11 @@
       <c r="F17" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1994</v>
       </c>
@@ -934,8 +982,9 @@
       <c r="F18" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1995</v>
       </c>
@@ -954,8 +1003,9 @@
       <c r="F19" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1996</v>
       </c>
@@ -974,6 +1024,7 @@
       <c r="F20" t="s">
         <v>55</v>
       </c>
+      <c r="G20" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>